<commit_message>
change in test scripts.
</commit_message>
<xml_diff>
--- a/tests/artifact/script/RestApi.xlsx
+++ b/tests/artifact/script/RestApi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6380" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6500" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2450,7 +2450,7 @@
     <t>And asserting whether the elapsed time is lesser than or eqals to 500milli seconds</t>
   </si>
   <si>
-    <t>500</t>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -6345,7 +6345,7 @@
   <dimension ref="A1:O189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
@@ -9874,8 +9874,5 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="F26" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated workflow for nexial
</commit_message>
<xml_diff>
--- a/tests/artifact/script/RestApi.xlsx
+++ b/tests/artifact/script/RestApi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6950" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6830" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -6347,7 +6347,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>

</xml_diff>